<commit_message>
Prescales: update pp reference prescales for menu v0_0_4 to fit in 100kHz rate budget
</commit_message>
<xml_diff>
--- a/Prescales/L1Menu_CollisionsPPRef2023_v0_0_4_0.xlsx
+++ b/Prescales/L1Menu_CollisionsPPRef2023_v0_0_4_0.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -492,7 +492,7 @@
         <v>17881</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2797</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
         <v>1</v>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
         <v>1</v>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" t="n">
         <v>1</v>
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
         <v>1</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="E76" t="n">
         <v>1</v>
@@ -1898,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E77" t="n">
         <v>1</v>
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" t="n">
         <v>1</v>
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108" t="n">
         <v>1</v>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" t="n">
         <v>1</v>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111" t="n">
         <v>1</v>
@@ -2563,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" t="n">
         <v>1</v>
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113" t="n">
         <v>1</v>
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E129" t="n">
         <v>1</v>
@@ -2905,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E130" t="n">
         <v>1</v>
@@ -3235,6 +3235,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prescales: change prescale for SingleJet24
</commit_message>
<xml_diff>
--- a/Prescales/L1Menu_CollisionsPPRef2023_v0_0_4_0.xlsx
+++ b/Prescales/L1Menu_CollisionsPPRef2023_v0_0_4_0.xlsx
@@ -2521,11 +2521,9 @@
           <t>L1_SingleJet24</t>
         </is>
       </c>
-      <c r="C110" t="n">
-        <v>0</v>
-      </c>
+      <c r="C110" t="inlineStr"/>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E110" t="n">
         <v>1</v>

</xml_diff>